<commit_message>
Last production tests at LPNHE
</commit_message>
<xml_diff>
--- a/Chips2000-2500Prod2017-02.xlsx
+++ b/Chips2000-2500Prod2017-02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="21180" windowHeight="10365" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="15" windowWidth="21180" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="29">
   <si>
     <t>PreScreening incidents</t>
   </si>
@@ -96,9 +96,6 @@
     <t>high noise</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>all channels stopped working</t>
   </si>
   <si>
@@ -112,7 +109,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,10 +190,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,9 +230,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -530,9 +540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J872"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,8 +629,8 @@
       <c r="C4" s="9"/>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
+      <c r="F4" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -683,8 +693,8 @@
       <c r="C8" s="9"/>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="3" t="s">
-        <v>26</v>
+      <c r="F8" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -795,8 +805,8 @@
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
+      <c r="F15" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -955,8 +965,8 @@
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="3" t="s">
-        <v>26</v>
+      <c r="F25" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -1195,8 +1205,8 @@
       <c r="C40" s="9"/>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="3" t="s">
-        <v>26</v>
+      <c r="F40" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -1243,8 +1253,8 @@
       <c r="C43" s="9"/>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="3" t="s">
-        <v>26</v>
+      <c r="F43" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -1307,8 +1317,8 @@
       <c r="C47" s="9"/>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="3" t="s">
-        <v>26</v>
+      <c r="F47" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -1387,8 +1397,8 @@
       <c r="C52" s="9"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="3" t="s">
-        <v>26</v>
+      <c r="F52" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -1749,7 +1759,7 @@
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J74" s="9"/>
     </row>
@@ -3041,7 +3051,7 @@
       <c r="D155" s="8"/>
       <c r="E155" s="9"/>
       <c r="F155" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G155" s="9"/>
       <c r="H155" s="9"/>
@@ -5552,7 +5562,9 @@
       <c r="C312" s="9"/>
       <c r="D312" s="9"/>
       <c r="E312" s="9"/>
-      <c r="F312" s="8"/>
+      <c r="F312" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G312" s="9"/>
       <c r="H312" s="9"/>
       <c r="I312" s="15"/>
@@ -5566,7 +5578,9 @@
       <c r="C313" s="9"/>
       <c r="D313" s="9"/>
       <c r="E313" s="9"/>
-      <c r="F313" s="8"/>
+      <c r="F313" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G313" s="9"/>
       <c r="H313" s="9"/>
       <c r="I313" s="14"/>
@@ -5580,7 +5594,9 @@
       <c r="C314" s="9"/>
       <c r="D314" s="9"/>
       <c r="E314" s="9"/>
-      <c r="F314" s="9"/>
+      <c r="F314" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G314" s="9"/>
       <c r="H314" s="9"/>
       <c r="I314" s="14"/>
@@ -5594,7 +5610,9 @@
       <c r="C315" s="9"/>
       <c r="D315" s="9"/>
       <c r="E315" s="9"/>
-      <c r="F315" s="8"/>
+      <c r="F315" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G315" s="9"/>
       <c r="H315" s="9"/>
       <c r="I315" s="15"/>
@@ -5608,7 +5626,9 @@
       <c r="C316" s="9"/>
       <c r="D316" s="9"/>
       <c r="E316" s="9"/>
-      <c r="F316" s="8"/>
+      <c r="F316" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G316" s="9"/>
       <c r="H316" s="9"/>
       <c r="I316" s="14"/>
@@ -5622,7 +5642,9 @@
       <c r="C317" s="9"/>
       <c r="D317" s="9"/>
       <c r="E317" s="9"/>
-      <c r="F317" s="8"/>
+      <c r="F317" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G317" s="9"/>
       <c r="H317" s="9"/>
       <c r="I317" s="14"/>
@@ -5636,7 +5658,9 @@
       <c r="C318" s="9"/>
       <c r="D318" s="9"/>
       <c r="E318" s="9"/>
-      <c r="F318" s="8"/>
+      <c r="F318" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G318" s="9"/>
       <c r="H318" s="9"/>
       <c r="I318" s="14"/>
@@ -5650,7 +5674,9 @@
       <c r="C319" s="9"/>
       <c r="D319" s="9"/>
       <c r="E319" s="9"/>
-      <c r="F319" s="8"/>
+      <c r="F319" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G319" s="9"/>
       <c r="H319" s="9"/>
       <c r="I319" s="14"/>
@@ -5664,7 +5690,9 @@
       <c r="C320" s="9"/>
       <c r="D320" s="9"/>
       <c r="E320" s="9"/>
-      <c r="F320" s="8"/>
+      <c r="F320" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G320" s="9"/>
       <c r="H320" s="9"/>
       <c r="I320" s="14"/>
@@ -5678,7 +5706,9 @@
       <c r="C321" s="9"/>
       <c r="D321" s="9"/>
       <c r="E321" s="9"/>
-      <c r="F321" s="8"/>
+      <c r="F321" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G321" s="9"/>
       <c r="H321" s="9"/>
       <c r="I321" s="15"/>
@@ -5692,7 +5722,9 @@
       <c r="C322" s="9"/>
       <c r="D322" s="9"/>
       <c r="E322" s="9"/>
-      <c r="F322" s="8"/>
+      <c r="F322" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G322" s="9"/>
       <c r="H322" s="9"/>
       <c r="I322" s="14"/>
@@ -5706,7 +5738,9 @@
       <c r="C323" s="9"/>
       <c r="D323" s="9"/>
       <c r="E323" s="9"/>
-      <c r="F323" s="8"/>
+      <c r="F323" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G323" s="9"/>
       <c r="H323" s="9"/>
       <c r="I323" s="14"/>
@@ -5720,7 +5754,9 @@
       <c r="C324" s="9"/>
       <c r="D324" s="9"/>
       <c r="E324" s="9"/>
-      <c r="F324" s="8"/>
+      <c r="F324" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G324" s="9"/>
       <c r="H324" s="9"/>
       <c r="I324" s="14"/>
@@ -5734,7 +5770,9 @@
       <c r="C325" s="9"/>
       <c r="D325" s="9"/>
       <c r="E325" s="9"/>
-      <c r="F325" s="9"/>
+      <c r="F325" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G325" s="9"/>
       <c r="H325" s="9"/>
       <c r="I325" s="14"/>
@@ -5748,7 +5786,9 @@
       <c r="C326" s="9"/>
       <c r="D326" s="9"/>
       <c r="E326" s="9"/>
-      <c r="F326" s="8"/>
+      <c r="F326" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G326" s="9"/>
       <c r="H326" s="9"/>
       <c r="I326" s="14"/>
@@ -5762,7 +5802,9 @@
       <c r="C327" s="9"/>
       <c r="D327" s="9"/>
       <c r="E327" s="9"/>
-      <c r="F327" s="9"/>
+      <c r="F327" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G327" s="9"/>
       <c r="H327" s="9"/>
       <c r="I327" s="14"/>
@@ -5776,7 +5818,9 @@
       <c r="C328" s="9"/>
       <c r="D328" s="9"/>
       <c r="E328" s="9"/>
-      <c r="F328" s="8"/>
+      <c r="F328" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G328" s="9"/>
       <c r="H328" s="9"/>
       <c r="I328" s="14"/>
@@ -5790,7 +5834,9 @@
       <c r="C329" s="9"/>
       <c r="D329" s="9"/>
       <c r="E329" s="9"/>
-      <c r="F329" s="8"/>
+      <c r="F329" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G329" s="9"/>
       <c r="H329" s="9"/>
       <c r="I329" s="14"/>
@@ -5804,7 +5850,9 @@
       <c r="C330" s="9"/>
       <c r="D330" s="9"/>
       <c r="E330" s="9"/>
-      <c r="F330" s="8"/>
+      <c r="F330" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G330" s="9"/>
       <c r="H330" s="9"/>
       <c r="I330" s="14"/>
@@ -5818,7 +5866,9 @@
       <c r="C331" s="9"/>
       <c r="D331" s="9"/>
       <c r="E331" s="9"/>
-      <c r="F331" s="8"/>
+      <c r="F331" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G331" s="9"/>
       <c r="H331" s="9"/>
       <c r="I331" s="15"/>
@@ -5832,7 +5882,9 @@
       <c r="C332" s="9"/>
       <c r="D332" s="9"/>
       <c r="E332" s="9"/>
-      <c r="F332" s="8"/>
+      <c r="F332" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G332" s="9"/>
       <c r="H332" s="9"/>
       <c r="I332" s="14"/>
@@ -5846,7 +5898,9 @@
       <c r="C333" s="9"/>
       <c r="D333" s="9"/>
       <c r="E333" s="9"/>
-      <c r="F333" s="8"/>
+      <c r="F333" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G333" s="9"/>
       <c r="H333" s="9"/>
       <c r="I333" s="14"/>
@@ -5860,7 +5914,9 @@
       <c r="C334" s="9"/>
       <c r="D334" s="9"/>
       <c r="E334" s="9"/>
-      <c r="F334" s="8"/>
+      <c r="F334" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G334" s="9"/>
       <c r="H334" s="9"/>
       <c r="I334" s="14"/>
@@ -5874,7 +5930,9 @@
       <c r="C335" s="9"/>
       <c r="D335" s="9"/>
       <c r="E335" s="9"/>
-      <c r="F335" s="8"/>
+      <c r="F335" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G335" s="9"/>
       <c r="H335" s="9"/>
       <c r="I335" s="15"/>
@@ -5888,7 +5946,9 @@
       <c r="C336" s="9"/>
       <c r="D336" s="9"/>
       <c r="E336" s="9"/>
-      <c r="F336" s="8"/>
+      <c r="F336" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G336" s="9"/>
       <c r="H336" s="9"/>
       <c r="I336" s="14"/>
@@ -5902,7 +5962,9 @@
       <c r="C337" s="9"/>
       <c r="D337" s="9"/>
       <c r="E337" s="9"/>
-      <c r="F337" s="8"/>
+      <c r="F337" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G337" s="9"/>
       <c r="H337" s="9"/>
       <c r="I337" s="14"/>
@@ -5916,7 +5978,9 @@
       <c r="C338" s="9"/>
       <c r="D338" s="9"/>
       <c r="E338" s="9"/>
-      <c r="F338" s="8"/>
+      <c r="F338" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G338" s="9"/>
       <c r="H338" s="9"/>
       <c r="I338" s="14"/>
@@ -5930,7 +5994,9 @@
       <c r="C339" s="9"/>
       <c r="D339" s="9"/>
       <c r="E339" s="9"/>
-      <c r="F339" s="8"/>
+      <c r="F339" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G339" s="9"/>
       <c r="H339" s="9"/>
       <c r="I339" s="14"/>
@@ -5944,7 +6010,9 @@
       <c r="C340" s="9"/>
       <c r="D340" s="9"/>
       <c r="E340" s="9"/>
-      <c r="F340" s="8"/>
+      <c r="F340" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G340" s="9"/>
       <c r="H340" s="9"/>
       <c r="I340" s="14"/>
@@ -5958,7 +6026,9 @@
       <c r="C341" s="9"/>
       <c r="D341" s="9"/>
       <c r="E341" s="9"/>
-      <c r="F341" s="8"/>
+      <c r="F341" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="G341" s="9"/>
       <c r="H341" s="9"/>
       <c r="I341" s="14"/>
@@ -5972,7 +6042,9 @@
       <c r="C342" s="9"/>
       <c r="D342" s="9"/>
       <c r="E342" s="9"/>
-      <c r="F342" s="9"/>
+      <c r="F342" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G342" s="9"/>
       <c r="H342" s="9"/>
       <c r="I342" s="14"/>
@@ -5986,7 +6058,9 @@
       <c r="C343" s="9"/>
       <c r="D343" s="9"/>
       <c r="E343" s="9"/>
-      <c r="F343" s="8"/>
+      <c r="F343" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G343" s="9"/>
       <c r="H343" s="9"/>
       <c r="I343" s="14"/>
@@ -6000,7 +6074,9 @@
       <c r="C344" s="9"/>
       <c r="D344" s="9"/>
       <c r="E344" s="9"/>
-      <c r="F344" s="8"/>
+      <c r="F344" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G344" s="9"/>
       <c r="H344" s="9"/>
       <c r="I344" s="14"/>
@@ -6014,7 +6090,9 @@
       <c r="C345" s="9"/>
       <c r="D345" s="9"/>
       <c r="E345" s="9"/>
-      <c r="F345" s="8"/>
+      <c r="F345" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G345" s="9"/>
       <c r="H345" s="9"/>
       <c r="I345" s="14"/>
@@ -6028,7 +6106,9 @@
       <c r="C346" s="9"/>
       <c r="D346" s="9"/>
       <c r="E346" s="9"/>
-      <c r="F346" s="8"/>
+      <c r="F346" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G346" s="9"/>
       <c r="H346" s="9"/>
       <c r="I346" s="14"/>
@@ -6042,7 +6122,9 @@
       <c r="C347" s="9"/>
       <c r="D347" s="9"/>
       <c r="E347" s="9"/>
-      <c r="F347" s="8"/>
+      <c r="F347" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G347" s="9"/>
       <c r="H347" s="9"/>
       <c r="I347" s="14"/>
@@ -6056,7 +6138,9 @@
       <c r="C348" s="9"/>
       <c r="D348" s="9"/>
       <c r="E348" s="9"/>
-      <c r="F348" s="8"/>
+      <c r="F348" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G348" s="9"/>
       <c r="H348" s="9"/>
       <c r="I348" s="15"/>
@@ -6070,7 +6154,9 @@
       <c r="C349" s="9"/>
       <c r="D349" s="9"/>
       <c r="E349" s="9"/>
-      <c r="F349" s="8"/>
+      <c r="F349" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G349" s="9"/>
       <c r="H349" s="9"/>
       <c r="I349" s="15"/>
@@ -6084,7 +6170,9 @@
       <c r="C350" s="9"/>
       <c r="D350" s="9"/>
       <c r="E350" s="9"/>
-      <c r="F350" s="9"/>
+      <c r="F350" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G350" s="9"/>
       <c r="H350" s="9"/>
       <c r="I350" s="14"/>
@@ -6098,7 +6186,9 @@
       <c r="C351" s="9"/>
       <c r="D351" s="9"/>
       <c r="E351" s="9"/>
-      <c r="F351" s="9"/>
+      <c r="F351" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G351" s="9"/>
       <c r="H351" s="9"/>
       <c r="I351" s="14"/>
@@ -6112,7 +6202,9 @@
       <c r="C352" s="9"/>
       <c r="D352" s="9"/>
       <c r="E352" s="9"/>
-      <c r="F352" s="9"/>
+      <c r="F352" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G352" s="9"/>
       <c r="H352" s="9"/>
       <c r="I352" s="14"/>
@@ -6126,7 +6218,9 @@
       <c r="C353" s="9"/>
       <c r="D353" s="9"/>
       <c r="E353" s="9"/>
-      <c r="F353" s="9"/>
+      <c r="F353" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G353" s="9"/>
       <c r="H353" s="9"/>
       <c r="I353" s="14"/>
@@ -6140,7 +6234,9 @@
       <c r="C354" s="9"/>
       <c r="D354" s="9"/>
       <c r="E354" s="9"/>
-      <c r="F354" s="9"/>
+      <c r="F354" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G354" s="9"/>
       <c r="H354" s="9"/>
       <c r="I354" s="14"/>
@@ -6154,7 +6250,9 @@
       <c r="C355" s="9"/>
       <c r="D355" s="9"/>
       <c r="E355" s="9"/>
-      <c r="F355" s="9"/>
+      <c r="F355" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G355" s="9"/>
       <c r="H355" s="9"/>
       <c r="I355" s="14"/>
@@ -6168,7 +6266,9 @@
       <c r="C356" s="9"/>
       <c r="D356" s="9"/>
       <c r="E356" s="9"/>
-      <c r="F356" s="9"/>
+      <c r="F356" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G356" s="9"/>
       <c r="H356" s="9"/>
       <c r="I356" s="14"/>
@@ -6182,7 +6282,9 @@
       <c r="C357" s="9"/>
       <c r="D357" s="9"/>
       <c r="E357" s="9"/>
-      <c r="F357" s="9"/>
+      <c r="F357" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G357" s="9"/>
       <c r="H357" s="9"/>
       <c r="I357" s="14"/>
@@ -6196,7 +6298,9 @@
       <c r="C358" s="9"/>
       <c r="D358" s="9"/>
       <c r="E358" s="9"/>
-      <c r="F358" s="9"/>
+      <c r="F358" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G358" s="9"/>
       <c r="H358" s="9"/>
       <c r="I358" s="14"/>
@@ -6210,7 +6314,9 @@
       <c r="C359" s="9"/>
       <c r="D359" s="9"/>
       <c r="E359" s="9"/>
-      <c r="F359" s="9"/>
+      <c r="F359" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G359" s="9"/>
       <c r="H359" s="9"/>
       <c r="I359" s="14"/>
@@ -6224,7 +6330,9 @@
       <c r="C360" s="9"/>
       <c r="D360" s="9"/>
       <c r="E360" s="9"/>
-      <c r="F360" s="9"/>
+      <c r="F360" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G360" s="9"/>
       <c r="H360" s="9"/>
       <c r="I360" s="14"/>
@@ -6238,7 +6346,9 @@
       <c r="C361" s="9"/>
       <c r="D361" s="9"/>
       <c r="E361" s="9"/>
-      <c r="F361" s="9"/>
+      <c r="F361" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G361" s="9"/>
       <c r="H361" s="9"/>
       <c r="I361" s="14"/>
@@ -6252,7 +6362,9 @@
       <c r="C362" s="9"/>
       <c r="D362" s="9"/>
       <c r="E362" s="9"/>
-      <c r="F362" s="9"/>
+      <c r="F362" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G362" s="9"/>
       <c r="H362" s="9"/>
       <c r="I362" s="14"/>
@@ -6266,7 +6378,9 @@
       <c r="C363" s="9"/>
       <c r="D363" s="9"/>
       <c r="E363" s="9"/>
-      <c r="F363" s="9"/>
+      <c r="F363" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G363" s="9"/>
       <c r="H363" s="9"/>
       <c r="I363" s="14"/>
@@ -6280,7 +6394,9 @@
       <c r="C364" s="9"/>
       <c r="D364" s="9"/>
       <c r="E364" s="9"/>
-      <c r="F364" s="9"/>
+      <c r="F364" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G364" s="9"/>
       <c r="H364" s="9"/>
       <c r="I364" s="14"/>
@@ -6294,7 +6410,9 @@
       <c r="C365" s="9"/>
       <c r="D365" s="9"/>
       <c r="E365" s="9"/>
-      <c r="F365" s="9"/>
+      <c r="F365" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G365" s="9"/>
       <c r="H365" s="9"/>
       <c r="I365" s="14"/>
@@ -6308,7 +6426,9 @@
       <c r="C366" s="9"/>
       <c r="D366" s="9"/>
       <c r="E366" s="9"/>
-      <c r="F366" s="9"/>
+      <c r="F366" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G366" s="9"/>
       <c r="H366" s="9"/>
       <c r="I366" s="14"/>
@@ -6322,7 +6442,9 @@
       <c r="C367" s="9"/>
       <c r="D367" s="9"/>
       <c r="E367" s="9"/>
-      <c r="F367" s="9"/>
+      <c r="F367" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G367" s="9"/>
       <c r="H367" s="9"/>
       <c r="I367" s="14"/>
@@ -6336,7 +6458,9 @@
       <c r="C368" s="9"/>
       <c r="D368" s="9"/>
       <c r="E368" s="9"/>
-      <c r="F368" s="9"/>
+      <c r="F368" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G368" s="9"/>
       <c r="H368" s="9"/>
       <c r="I368" s="14"/>
@@ -6350,7 +6474,9 @@
       <c r="C369" s="9"/>
       <c r="D369" s="9"/>
       <c r="E369" s="9"/>
-      <c r="F369" s="9"/>
+      <c r="F369" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G369" s="9"/>
       <c r="H369" s="9"/>
       <c r="I369" s="14"/>
@@ -6364,7 +6490,9 @@
       <c r="C370" s="9"/>
       <c r="D370" s="9"/>
       <c r="E370" s="9"/>
-      <c r="F370" s="9"/>
+      <c r="F370" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G370" s="9"/>
       <c r="H370" s="9"/>
       <c r="I370" s="14"/>
@@ -6378,7 +6506,9 @@
       <c r="C371" s="9"/>
       <c r="D371" s="9"/>
       <c r="E371" s="9"/>
-      <c r="F371" s="9"/>
+      <c r="F371" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G371" s="9"/>
       <c r="H371" s="9"/>
       <c r="I371" s="14"/>
@@ -6392,7 +6522,9 @@
       <c r="C372" s="9"/>
       <c r="D372" s="9"/>
       <c r="E372" s="9"/>
-      <c r="F372" s="9"/>
+      <c r="F372" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G372" s="9"/>
       <c r="H372" s="9"/>
       <c r="I372" s="14"/>
@@ -6406,7 +6538,9 @@
       <c r="C373" s="9"/>
       <c r="D373" s="9"/>
       <c r="E373" s="9"/>
-      <c r="F373" s="9"/>
+      <c r="F373" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G373" s="9"/>
       <c r="H373" s="9"/>
       <c r="I373" s="14"/>
@@ -6420,7 +6554,9 @@
       <c r="C374" s="9"/>
       <c r="D374" s="9"/>
       <c r="E374" s="9"/>
-      <c r="F374" s="9"/>
+      <c r="F374" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G374" s="9"/>
       <c r="H374" s="9"/>
       <c r="I374" s="14"/>
@@ -6434,7 +6570,9 @@
       <c r="C375" s="9"/>
       <c r="D375" s="9"/>
       <c r="E375" s="9"/>
-      <c r="F375" s="9"/>
+      <c r="F375" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G375" s="9"/>
       <c r="H375" s="9"/>
       <c r="I375" s="14"/>
@@ -6448,7 +6586,9 @@
       <c r="C376" s="9"/>
       <c r="D376" s="9"/>
       <c r="E376" s="9"/>
-      <c r="F376" s="9"/>
+      <c r="F376" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G376" s="9"/>
       <c r="H376" s="9"/>
       <c r="I376" s="14"/>
@@ -6462,7 +6602,9 @@
       <c r="C377" s="9"/>
       <c r="D377" s="9"/>
       <c r="E377" s="9"/>
-      <c r="F377" s="9"/>
+      <c r="F377" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G377" s="9"/>
       <c r="H377" s="9"/>
       <c r="I377" s="14"/>
@@ -6476,7 +6618,9 @@
       <c r="C378" s="9"/>
       <c r="D378" s="9"/>
       <c r="E378" s="9"/>
-      <c r="F378" s="9"/>
+      <c r="F378" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G378" s="9"/>
       <c r="H378" s="9"/>
       <c r="I378" s="14"/>
@@ -6490,7 +6634,9 @@
       <c r="C379" s="9"/>
       <c r="D379" s="9"/>
       <c r="E379" s="9"/>
-      <c r="F379" s="9"/>
+      <c r="F379" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G379" s="9"/>
       <c r="H379" s="9"/>
       <c r="I379" s="14"/>
@@ -6504,7 +6650,9 @@
       <c r="C380" s="9"/>
       <c r="D380" s="9"/>
       <c r="E380" s="9"/>
-      <c r="F380" s="9"/>
+      <c r="F380" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G380" s="9"/>
       <c r="H380" s="9"/>
       <c r="I380" s="14"/>
@@ -6518,7 +6666,9 @@
       <c r="C381" s="9"/>
       <c r="D381" s="9"/>
       <c r="E381" s="9"/>
-      <c r="F381" s="9"/>
+      <c r="F381" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G381" s="9"/>
       <c r="H381" s="9"/>
       <c r="I381" s="14"/>
@@ -6532,7 +6682,9 @@
       <c r="C382" s="9"/>
       <c r="D382" s="9"/>
       <c r="E382" s="9"/>
-      <c r="F382" s="9"/>
+      <c r="F382" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G382" s="9"/>
       <c r="H382" s="9"/>
       <c r="I382" s="14"/>
@@ -6546,7 +6698,9 @@
       <c r="C383" s="9"/>
       <c r="D383" s="9"/>
       <c r="E383" s="9"/>
-      <c r="F383" s="9"/>
+      <c r="F383" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G383" s="9"/>
       <c r="H383" s="9"/>
       <c r="I383" s="14"/>
@@ -6560,7 +6714,9 @@
       <c r="C384" s="9"/>
       <c r="D384" s="9"/>
       <c r="E384" s="9"/>
-      <c r="F384" s="9"/>
+      <c r="F384" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G384" s="9"/>
       <c r="H384" s="9"/>
       <c r="I384" s="14"/>
@@ -6574,7 +6730,9 @@
       <c r="C385" s="9"/>
       <c r="D385" s="9"/>
       <c r="E385" s="9"/>
-      <c r="F385" s="9"/>
+      <c r="F385" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G385" s="9"/>
       <c r="H385" s="9"/>
       <c r="I385" s="14"/>
@@ -6588,7 +6746,9 @@
       <c r="C386" s="9"/>
       <c r="D386" s="9"/>
       <c r="E386" s="9"/>
-      <c r="F386" s="9"/>
+      <c r="F386" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G386" s="9"/>
       <c r="H386" s="9"/>
       <c r="I386" s="14"/>
@@ -6602,7 +6762,9 @@
       <c r="C387" s="9"/>
       <c r="D387" s="9"/>
       <c r="E387" s="9"/>
-      <c r="F387" s="9"/>
+      <c r="F387" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G387" s="9"/>
       <c r="H387" s="9"/>
       <c r="I387" s="14"/>
@@ -6616,7 +6778,9 @@
       <c r="C388" s="9"/>
       <c r="D388" s="9"/>
       <c r="E388" s="9"/>
-      <c r="F388" s="9"/>
+      <c r="F388" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G388" s="9"/>
       <c r="H388" s="9"/>
       <c r="I388" s="14"/>
@@ -6630,7 +6794,9 @@
       <c r="C389" s="9"/>
       <c r="D389" s="9"/>
       <c r="E389" s="9"/>
-      <c r="F389" s="9"/>
+      <c r="F389" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G389" s="9"/>
       <c r="H389" s="9"/>
       <c r="I389" s="14"/>
@@ -6644,7 +6810,9 @@
       <c r="C390" s="9"/>
       <c r="D390" s="9"/>
       <c r="E390" s="9"/>
-      <c r="F390" s="9"/>
+      <c r="F390" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G390" s="9"/>
       <c r="H390" s="9"/>
       <c r="I390" s="14"/>
@@ -6658,7 +6826,9 @@
       <c r="C391" s="9"/>
       <c r="D391" s="9"/>
       <c r="E391" s="9"/>
-      <c r="F391" s="9"/>
+      <c r="F391" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G391" s="9"/>
       <c r="H391" s="9"/>
       <c r="I391" s="14"/>
@@ -6672,7 +6842,9 @@
       <c r="C392" s="9"/>
       <c r="D392" s="9"/>
       <c r="E392" s="9"/>
-      <c r="F392" s="9"/>
+      <c r="F392" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G392" s="9"/>
       <c r="H392" s="9"/>
       <c r="I392" s="14"/>
@@ -6686,7 +6858,9 @@
       <c r="C393" s="9"/>
       <c r="D393" s="9"/>
       <c r="E393" s="9"/>
-      <c r="F393" s="9"/>
+      <c r="F393" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G393" s="9"/>
       <c r="H393" s="9"/>
       <c r="I393" s="14"/>
@@ -6700,7 +6874,9 @@
       <c r="C394" s="9"/>
       <c r="D394" s="9"/>
       <c r="E394" s="9"/>
-      <c r="F394" s="9"/>
+      <c r="F394" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G394" s="9"/>
       <c r="H394" s="9"/>
       <c r="I394" s="14"/>
@@ -6714,7 +6890,9 @@
       <c r="C395" s="9"/>
       <c r="D395" s="9"/>
       <c r="E395" s="9"/>
-      <c r="F395" s="9"/>
+      <c r="F395" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G395" s="9"/>
       <c r="H395" s="9"/>
       <c r="I395" s="14"/>
@@ -6728,7 +6906,9 @@
       <c r="C396" s="9"/>
       <c r="D396" s="9"/>
       <c r="E396" s="9"/>
-      <c r="F396" s="9"/>
+      <c r="F396" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G396" s="9"/>
       <c r="H396" s="9"/>
       <c r="I396" s="14"/>
@@ -6742,7 +6922,9 @@
       <c r="C397" s="9"/>
       <c r="D397" s="9"/>
       <c r="E397" s="9"/>
-      <c r="F397" s="9"/>
+      <c r="F397" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G397" s="9"/>
       <c r="H397" s="9"/>
       <c r="I397" s="14"/>
@@ -6756,7 +6938,9 @@
       <c r="C398" s="9"/>
       <c r="D398" s="9"/>
       <c r="E398" s="9"/>
-      <c r="F398" s="9"/>
+      <c r="F398" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G398" s="9"/>
       <c r="H398" s="9"/>
       <c r="I398" s="14"/>
@@ -6770,7 +6954,9 @@
       <c r="C399" s="9"/>
       <c r="D399" s="9"/>
       <c r="E399" s="9"/>
-      <c r="F399" s="9"/>
+      <c r="F399" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G399" s="9"/>
       <c r="H399" s="9"/>
       <c r="I399" s="14"/>
@@ -6784,7 +6970,9 @@
       <c r="C400" s="9"/>
       <c r="D400" s="9"/>
       <c r="E400" s="9"/>
-      <c r="F400" s="9"/>
+      <c r="F400" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G400" s="9"/>
       <c r="H400" s="9"/>
       <c r="I400" s="14"/>
@@ -6798,7 +6986,9 @@
       <c r="C401" s="9"/>
       <c r="D401" s="9"/>
       <c r="E401" s="9"/>
-      <c r="F401" s="9"/>
+      <c r="F401" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G401" s="9"/>
       <c r="H401" s="9"/>
       <c r="I401" s="14"/>
@@ -6812,7 +7002,9 @@
       <c r="C402" s="9"/>
       <c r="D402" s="9"/>
       <c r="E402" s="9"/>
-      <c r="F402" s="9"/>
+      <c r="F402" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G402" s="9"/>
       <c r="H402" s="9"/>
       <c r="I402" s="14"/>
@@ -6826,7 +7018,9 @@
       <c r="C403" s="9"/>
       <c r="D403" s="9"/>
       <c r="E403" s="9"/>
-      <c r="F403" s="9"/>
+      <c r="F403" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G403" s="9"/>
       <c r="H403" s="9"/>
       <c r="I403" s="14"/>
@@ -6840,7 +7034,9 @@
       <c r="C404" s="9"/>
       <c r="D404" s="9"/>
       <c r="E404" s="9"/>
-      <c r="F404" s="9"/>
+      <c r="F404" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G404" s="9"/>
       <c r="H404" s="9"/>
       <c r="I404" s="14"/>
@@ -6854,7 +7050,9 @@
       <c r="C405" s="9"/>
       <c r="D405" s="9"/>
       <c r="E405" s="9"/>
-      <c r="F405" s="9"/>
+      <c r="F405" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G405" s="9"/>
       <c r="H405" s="9"/>
       <c r="I405" s="14"/>
@@ -6868,7 +7066,9 @@
       <c r="C406" s="9"/>
       <c r="D406" s="9"/>
       <c r="E406" s="9"/>
-      <c r="F406" s="9"/>
+      <c r="F406" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G406" s="9"/>
       <c r="H406" s="9"/>
       <c r="I406" s="14"/>
@@ -6882,7 +7082,9 @@
       <c r="C407" s="9"/>
       <c r="D407" s="9"/>
       <c r="E407" s="9"/>
-      <c r="F407" s="9"/>
+      <c r="F407" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G407" s="9"/>
       <c r="H407" s="9"/>
       <c r="I407" s="14"/>
@@ -6896,7 +7098,9 @@
       <c r="C408" s="9"/>
       <c r="D408" s="9"/>
       <c r="E408" s="9"/>
-      <c r="F408" s="9"/>
+      <c r="F408" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G408" s="9"/>
       <c r="H408" s="9"/>
       <c r="I408" s="14"/>
@@ -6910,7 +7114,9 @@
       <c r="C409" s="9"/>
       <c r="D409" s="9"/>
       <c r="E409" s="9"/>
-      <c r="F409" s="9"/>
+      <c r="F409" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G409" s="9"/>
       <c r="H409" s="9"/>
       <c r="I409" s="14"/>
@@ -6924,7 +7130,9 @@
       <c r="C410" s="9"/>
       <c r="D410" s="9"/>
       <c r="E410" s="9"/>
-      <c r="F410" s="9"/>
+      <c r="F410" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G410" s="9"/>
       <c r="H410" s="9"/>
       <c r="I410" s="14"/>
@@ -6938,7 +7146,9 @@
       <c r="C411" s="9"/>
       <c r="D411" s="9"/>
       <c r="E411" s="9"/>
-      <c r="F411" s="9"/>
+      <c r="F411" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G411" s="9"/>
       <c r="H411" s="9"/>
       <c r="I411" s="14"/>
@@ -6952,7 +7162,9 @@
       <c r="C412" s="9"/>
       <c r="D412" s="9"/>
       <c r="E412" s="9"/>
-      <c r="F412" s="9"/>
+      <c r="F412" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G412" s="9"/>
       <c r="H412" s="9"/>
       <c r="I412" s="14"/>
@@ -6966,7 +7178,9 @@
       <c r="C413" s="9"/>
       <c r="D413" s="9"/>
       <c r="E413" s="9"/>
-      <c r="F413" s="9"/>
+      <c r="F413" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G413" s="9"/>
       <c r="H413" s="9"/>
       <c r="I413" s="14"/>
@@ -6980,7 +7194,9 @@
       <c r="C414" s="9"/>
       <c r="D414" s="9"/>
       <c r="E414" s="9"/>
-      <c r="F414" s="9"/>
+      <c r="F414" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G414" s="9"/>
       <c r="H414" s="9"/>
       <c r="I414" s="14"/>
@@ -6994,7 +7210,9 @@
       <c r="C415" s="9"/>
       <c r="D415" s="9"/>
       <c r="E415" s="9"/>
-      <c r="F415" s="9"/>
+      <c r="F415" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G415" s="9"/>
       <c r="H415" s="9"/>
       <c r="I415" s="14"/>
@@ -7008,7 +7226,9 @@
       <c r="C416" s="9"/>
       <c r="D416" s="9"/>
       <c r="E416" s="9"/>
-      <c r="F416" s="9"/>
+      <c r="F416" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G416" s="9"/>
       <c r="H416" s="9"/>
       <c r="I416" s="14"/>
@@ -7022,7 +7242,9 @@
       <c r="C417" s="9"/>
       <c r="D417" s="9"/>
       <c r="E417" s="9"/>
-      <c r="F417" s="9"/>
+      <c r="F417" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G417" s="9"/>
       <c r="H417" s="9"/>
       <c r="I417" s="14"/>
@@ -7036,7 +7258,9 @@
       <c r="C418" s="9"/>
       <c r="D418" s="9"/>
       <c r="E418" s="9"/>
-      <c r="F418" s="9"/>
+      <c r="F418" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G418" s="9"/>
       <c r="H418" s="9"/>
       <c r="I418" s="14"/>
@@ -7050,7 +7274,9 @@
       <c r="C419" s="9"/>
       <c r="D419" s="9"/>
       <c r="E419" s="9"/>
-      <c r="F419" s="9"/>
+      <c r="F419" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G419" s="9"/>
       <c r="H419" s="9"/>
       <c r="I419" s="14"/>
@@ -7064,7 +7290,9 @@
       <c r="C420" s="9"/>
       <c r="D420" s="9"/>
       <c r="E420" s="9"/>
-      <c r="F420" s="9"/>
+      <c r="F420" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G420" s="9"/>
       <c r="H420" s="9"/>
       <c r="I420" s="14"/>
@@ -7078,7 +7306,9 @@
       <c r="C421" s="9"/>
       <c r="D421" s="9"/>
       <c r="E421" s="9"/>
-      <c r="F421" s="9"/>
+      <c r="F421" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G421" s="9"/>
       <c r="H421" s="9"/>
       <c r="I421" s="14"/>
@@ -7092,7 +7322,9 @@
       <c r="C422" s="9"/>
       <c r="D422" s="9"/>
       <c r="E422" s="9"/>
-      <c r="F422" s="9"/>
+      <c r="F422" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G422" s="9"/>
       <c r="H422" s="9"/>
       <c r="I422" s="14"/>
@@ -7106,7 +7338,9 @@
       <c r="C423" s="9"/>
       <c r="D423" s="9"/>
       <c r="E423" s="9"/>
-      <c r="F423" s="9"/>
+      <c r="F423" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G423" s="9"/>
       <c r="H423" s="9"/>
       <c r="I423" s="14"/>
@@ -7120,7 +7354,9 @@
       <c r="C424" s="9"/>
       <c r="D424" s="9"/>
       <c r="E424" s="9"/>
-      <c r="F424" s="9"/>
+      <c r="F424" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G424" s="9"/>
       <c r="H424" s="9"/>
       <c r="I424" s="14"/>
@@ -7134,7 +7370,9 @@
       <c r="C425" s="9"/>
       <c r="D425" s="9"/>
       <c r="E425" s="9"/>
-      <c r="F425" s="9"/>
+      <c r="F425" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G425" s="9"/>
       <c r="H425" s="9"/>
       <c r="I425" s="14"/>
@@ -7148,7 +7386,9 @@
       <c r="C426" s="9"/>
       <c r="D426" s="9"/>
       <c r="E426" s="9"/>
-      <c r="F426" s="9"/>
+      <c r="F426" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G426" s="9"/>
       <c r="H426" s="9"/>
       <c r="I426" s="14"/>
@@ -7162,7 +7402,9 @@
       <c r="C427" s="9"/>
       <c r="D427" s="9"/>
       <c r="E427" s="9"/>
-      <c r="F427" s="9"/>
+      <c r="F427" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G427" s="9"/>
       <c r="H427" s="9"/>
       <c r="I427" s="14"/>
@@ -7176,7 +7418,9 @@
       <c r="C428" s="9"/>
       <c r="D428" s="9"/>
       <c r="E428" s="9"/>
-      <c r="F428" s="9"/>
+      <c r="F428" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G428" s="9"/>
       <c r="H428" s="9"/>
       <c r="I428" s="14"/>
@@ -7190,7 +7434,9 @@
       <c r="C429" s="9"/>
       <c r="D429" s="9"/>
       <c r="E429" s="9"/>
-      <c r="F429" s="9"/>
+      <c r="F429" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G429" s="9"/>
       <c r="H429" s="9"/>
       <c r="I429" s="14"/>
@@ -7204,7 +7450,9 @@
       <c r="C430" s="9"/>
       <c r="D430" s="9"/>
       <c r="E430" s="9"/>
-      <c r="F430" s="9"/>
+      <c r="F430" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G430" s="9"/>
       <c r="H430" s="9"/>
       <c r="I430" s="14"/>
@@ -7218,7 +7466,9 @@
       <c r="C431" s="9"/>
       <c r="D431" s="9"/>
       <c r="E431" s="9"/>
-      <c r="F431" s="9"/>
+      <c r="F431" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G431" s="9"/>
       <c r="H431" s="9"/>
       <c r="I431" s="14"/>
@@ -7232,7 +7482,9 @@
       <c r="C432" s="9"/>
       <c r="D432" s="9"/>
       <c r="E432" s="9"/>
-      <c r="F432" s="9"/>
+      <c r="F432" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G432" s="9"/>
       <c r="H432" s="9"/>
       <c r="I432" s="14"/>
@@ -7246,7 +7498,9 @@
       <c r="C433" s="9"/>
       <c r="D433" s="9"/>
       <c r="E433" s="9"/>
-      <c r="F433" s="9"/>
+      <c r="F433" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G433" s="9"/>
       <c r="H433" s="9"/>
       <c r="I433" s="14"/>
@@ -7260,7 +7514,9 @@
       <c r="C434" s="9"/>
       <c r="D434" s="9"/>
       <c r="E434" s="9"/>
-      <c r="F434" s="9"/>
+      <c r="F434" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G434" s="9"/>
       <c r="H434" s="9"/>
       <c r="I434" s="14"/>
@@ -7274,7 +7530,9 @@
       <c r="C435" s="9"/>
       <c r="D435" s="9"/>
       <c r="E435" s="9"/>
-      <c r="F435" s="9"/>
+      <c r="F435" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G435" s="9"/>
       <c r="H435" s="9"/>
       <c r="I435" s="14"/>
@@ -7288,7 +7546,9 @@
       <c r="C436" s="9"/>
       <c r="D436" s="9"/>
       <c r="E436" s="9"/>
-      <c r="F436" s="9"/>
+      <c r="F436" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G436" s="9"/>
       <c r="H436" s="9"/>
       <c r="I436" s="14"/>
@@ -7302,7 +7562,9 @@
       <c r="C437" s="9"/>
       <c r="D437" s="9"/>
       <c r="E437" s="9"/>
-      <c r="F437" s="9"/>
+      <c r="F437" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G437" s="9"/>
       <c r="H437" s="9"/>
       <c r="I437" s="14"/>
@@ -7316,7 +7578,9 @@
       <c r="C438" s="9"/>
       <c r="D438" s="9"/>
       <c r="E438" s="9"/>
-      <c r="F438" s="9"/>
+      <c r="F438" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G438" s="9"/>
       <c r="H438" s="9"/>
       <c r="I438" s="14"/>
@@ -7330,7 +7594,9 @@
       <c r="C439" s="9"/>
       <c r="D439" s="9"/>
       <c r="E439" s="9"/>
-      <c r="F439" s="9"/>
+      <c r="F439" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G439" s="9"/>
       <c r="H439" s="9"/>
       <c r="I439" s="14"/>
@@ -7344,7 +7610,9 @@
       <c r="C440" s="9"/>
       <c r="D440" s="9"/>
       <c r="E440" s="9"/>
-      <c r="F440" s="9"/>
+      <c r="F440" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G440" s="9"/>
       <c r="H440" s="9"/>
       <c r="I440" s="14"/>
@@ -7358,7 +7626,9 @@
       <c r="C441" s="9"/>
       <c r="D441" s="9"/>
       <c r="E441" s="9"/>
-      <c r="F441" s="9"/>
+      <c r="F441" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G441" s="9"/>
       <c r="H441" s="9"/>
       <c r="I441" s="14"/>
@@ -7372,7 +7642,9 @@
       <c r="C442" s="9"/>
       <c r="D442" s="9"/>
       <c r="E442" s="9"/>
-      <c r="F442" s="9"/>
+      <c r="F442" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G442" s="9"/>
       <c r="H442" s="9"/>
       <c r="I442" s="14"/>
@@ -7386,7 +7658,9 @@
       <c r="C443" s="9"/>
       <c r="D443" s="9"/>
       <c r="E443" s="9"/>
-      <c r="F443" s="9"/>
+      <c r="F443" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G443" s="9"/>
       <c r="H443" s="9"/>
       <c r="I443" s="14"/>
@@ -7400,7 +7674,9 @@
       <c r="C444" s="9"/>
       <c r="D444" s="9"/>
       <c r="E444" s="9"/>
-      <c r="F444" s="9"/>
+      <c r="F444" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G444" s="9"/>
       <c r="H444" s="9"/>
       <c r="I444" s="14"/>
@@ -7414,7 +7690,9 @@
       <c r="C445" s="9"/>
       <c r="D445" s="9"/>
       <c r="E445" s="9"/>
-      <c r="F445" s="9"/>
+      <c r="F445" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G445" s="9"/>
       <c r="H445" s="9"/>
       <c r="I445" s="14"/>
@@ -7428,7 +7706,9 @@
       <c r="C446" s="9"/>
       <c r="D446" s="9"/>
       <c r="E446" s="9"/>
-      <c r="F446" s="9"/>
+      <c r="F446" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G446" s="9"/>
       <c r="H446" s="9"/>
       <c r="I446" s="14"/>
@@ -7442,7 +7722,9 @@
       <c r="C447" s="9"/>
       <c r="D447" s="9"/>
       <c r="E447" s="9"/>
-      <c r="F447" s="9"/>
+      <c r="F447" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G447" s="9"/>
       <c r="H447" s="9"/>
       <c r="I447" s="14"/>
@@ -7456,7 +7738,9 @@
       <c r="C448" s="9"/>
       <c r="D448" s="9"/>
       <c r="E448" s="9"/>
-      <c r="F448" s="9"/>
+      <c r="F448" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G448" s="9"/>
       <c r="H448" s="9"/>
       <c r="I448" s="14"/>
@@ -7470,7 +7754,9 @@
       <c r="C449" s="9"/>
       <c r="D449" s="9"/>
       <c r="E449" s="9"/>
-      <c r="F449" s="9"/>
+      <c r="F449" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G449" s="9"/>
       <c r="H449" s="9"/>
       <c r="I449" s="14"/>
@@ -7484,7 +7770,9 @@
       <c r="C450" s="9"/>
       <c r="D450" s="9"/>
       <c r="E450" s="9"/>
-      <c r="F450" s="9"/>
+      <c r="F450" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G450" s="9"/>
       <c r="H450" s="9"/>
       <c r="I450" s="14"/>
@@ -7498,7 +7786,9 @@
       <c r="C451" s="9"/>
       <c r="D451" s="9"/>
       <c r="E451" s="9"/>
-      <c r="F451" s="9"/>
+      <c r="F451" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G451" s="9"/>
       <c r="H451" s="9"/>
       <c r="I451" s="14"/>
@@ -7512,7 +7802,9 @@
       <c r="C452" s="9"/>
       <c r="D452" s="9"/>
       <c r="E452" s="9"/>
-      <c r="F452" s="9"/>
+      <c r="F452" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G452" s="9"/>
       <c r="H452" s="9"/>
       <c r="I452" s="14"/>
@@ -7526,7 +7818,9 @@
       <c r="C453" s="9"/>
       <c r="D453" s="9"/>
       <c r="E453" s="9"/>
-      <c r="F453" s="9"/>
+      <c r="F453" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G453" s="9"/>
       <c r="H453" s="9"/>
       <c r="I453" s="14"/>
@@ -7540,7 +7834,9 @@
       <c r="C454" s="9"/>
       <c r="D454" s="9"/>
       <c r="E454" s="9"/>
-      <c r="F454" s="9"/>
+      <c r="F454" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G454" s="9"/>
       <c r="H454" s="9"/>
       <c r="I454" s="14"/>
@@ -7554,7 +7850,9 @@
       <c r="C455" s="9"/>
       <c r="D455" s="9"/>
       <c r="E455" s="9"/>
-      <c r="F455" s="9"/>
+      <c r="F455" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G455" s="9"/>
       <c r="H455" s="9"/>
       <c r="I455" s="14"/>
@@ -7568,7 +7866,9 @@
       <c r="C456" s="9"/>
       <c r="D456" s="9"/>
       <c r="E456" s="9"/>
-      <c r="F456" s="9"/>
+      <c r="F456" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G456" s="9"/>
       <c r="H456" s="9"/>
       <c r="I456" s="14"/>
@@ -7582,7 +7882,9 @@
       <c r="C457" s="9"/>
       <c r="D457" s="9"/>
       <c r="E457" s="9"/>
-      <c r="F457" s="9"/>
+      <c r="F457" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G457" s="9"/>
       <c r="H457" s="9"/>
       <c r="I457" s="14"/>
@@ -7596,7 +7898,9 @@
       <c r="C458" s="9"/>
       <c r="D458" s="9"/>
       <c r="E458" s="9"/>
-      <c r="F458" s="9"/>
+      <c r="F458" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G458" s="9"/>
       <c r="H458" s="9"/>
       <c r="I458" s="14"/>
@@ -7610,7 +7914,9 @@
       <c r="C459" s="9"/>
       <c r="D459" s="9"/>
       <c r="E459" s="9"/>
-      <c r="F459" s="9"/>
+      <c r="F459" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G459" s="9"/>
       <c r="H459" s="9"/>
       <c r="I459" s="14"/>
@@ -7624,7 +7930,9 @@
       <c r="C460" s="9"/>
       <c r="D460" s="9"/>
       <c r="E460" s="9"/>
-      <c r="F460" s="9"/>
+      <c r="F460" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G460" s="9"/>
       <c r="H460" s="9"/>
       <c r="I460" s="14"/>
@@ -7638,7 +7946,9 @@
       <c r="C461" s="9"/>
       <c r="D461" s="9"/>
       <c r="E461" s="9"/>
-      <c r="F461" s="9"/>
+      <c r="F461" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G461" s="9"/>
       <c r="H461" s="9"/>
       <c r="I461" s="14"/>
@@ -7652,7 +7962,9 @@
       <c r="C462" s="9"/>
       <c r="D462" s="9"/>
       <c r="E462" s="9"/>
-      <c r="F462" s="9"/>
+      <c r="F462" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G462" s="9"/>
       <c r="H462" s="9"/>
       <c r="I462" s="14"/>
@@ -7666,7 +7978,9 @@
       <c r="C463" s="9"/>
       <c r="D463" s="9"/>
       <c r="E463" s="9"/>
-      <c r="F463" s="9"/>
+      <c r="F463" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G463" s="9"/>
       <c r="H463" s="9"/>
       <c r="I463" s="14"/>
@@ -7680,7 +7994,9 @@
       <c r="C464" s="9"/>
       <c r="D464" s="9"/>
       <c r="E464" s="9"/>
-      <c r="F464" s="9"/>
+      <c r="F464" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G464" s="9"/>
       <c r="H464" s="9"/>
       <c r="I464" s="14"/>
@@ -7694,7 +8010,9 @@
       <c r="C465" s="9"/>
       <c r="D465" s="9"/>
       <c r="E465" s="9"/>
-      <c r="F465" s="9"/>
+      <c r="F465" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G465" s="9"/>
       <c r="H465" s="9"/>
       <c r="I465" s="14"/>
@@ -7708,7 +8026,9 @@
       <c r="C466" s="9"/>
       <c r="D466" s="9"/>
       <c r="E466" s="9"/>
-      <c r="F466" s="9"/>
+      <c r="F466" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G466" s="9"/>
       <c r="H466" s="9"/>
       <c r="I466" s="14"/>
@@ -7722,7 +8042,9 @@
       <c r="C467" s="9"/>
       <c r="D467" s="9"/>
       <c r="E467" s="9"/>
-      <c r="F467" s="9"/>
+      <c r="F467" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G467" s="9"/>
       <c r="H467" s="9"/>
       <c r="I467" s="14"/>
@@ -7736,7 +8058,9 @@
       <c r="C468" s="9"/>
       <c r="D468" s="9"/>
       <c r="E468" s="9"/>
-      <c r="F468" s="9"/>
+      <c r="F468" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G468" s="9"/>
       <c r="H468" s="9"/>
       <c r="I468" s="14"/>
@@ -7750,7 +8074,9 @@
       <c r="C469" s="9"/>
       <c r="D469" s="9"/>
       <c r="E469" s="9"/>
-      <c r="F469" s="9"/>
+      <c r="F469" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G469" s="9"/>
       <c r="H469" s="9"/>
       <c r="I469" s="14"/>
@@ -7764,7 +8090,9 @@
       <c r="C470" s="9"/>
       <c r="D470" s="9"/>
       <c r="E470" s="9"/>
-      <c r="F470" s="9"/>
+      <c r="F470" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G470" s="9"/>
       <c r="H470" s="9"/>
       <c r="I470" s="14"/>
@@ -7778,7 +8106,9 @@
       <c r="C471" s="9"/>
       <c r="D471" s="9"/>
       <c r="E471" s="9"/>
-      <c r="F471" s="9"/>
+      <c r="F471" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G471" s="9"/>
       <c r="H471" s="9"/>
       <c r="I471" s="14"/>
@@ -7792,7 +8122,9 @@
       <c r="C472" s="9"/>
       <c r="D472" s="9"/>
       <c r="E472" s="9"/>
-      <c r="F472" s="9"/>
+      <c r="F472" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G472" s="9"/>
       <c r="H472" s="9"/>
       <c r="I472" s="14"/>
@@ -7806,7 +8138,9 @@
       <c r="C473" s="9"/>
       <c r="D473" s="9"/>
       <c r="E473" s="9"/>
-      <c r="F473" s="9"/>
+      <c r="F473" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G473" s="9"/>
       <c r="H473" s="9"/>
       <c r="I473" s="14"/>
@@ -7820,7 +8154,9 @@
       <c r="C474" s="9"/>
       <c r="D474" s="9"/>
       <c r="E474" s="9"/>
-      <c r="F474" s="9"/>
+      <c r="F474" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G474" s="9"/>
       <c r="H474" s="9"/>
       <c r="I474" s="14"/>
@@ -7834,7 +8170,9 @@
       <c r="C475" s="9"/>
       <c r="D475" s="9"/>
       <c r="E475" s="9"/>
-      <c r="F475" s="9"/>
+      <c r="F475" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G475" s="9"/>
       <c r="H475" s="9"/>
       <c r="I475" s="14"/>
@@ -7848,7 +8186,9 @@
       <c r="C476" s="9"/>
       <c r="D476" s="9"/>
       <c r="E476" s="9"/>
-      <c r="F476" s="9"/>
+      <c r="F476" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G476" s="9"/>
       <c r="H476" s="9"/>
       <c r="I476" s="14"/>
@@ -7862,7 +8202,9 @@
       <c r="C477" s="9"/>
       <c r="D477" s="9"/>
       <c r="E477" s="9"/>
-      <c r="F477" s="9"/>
+      <c r="F477" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G477" s="9"/>
       <c r="H477" s="9"/>
       <c r="I477" s="14"/>
@@ -7876,7 +8218,9 @@
       <c r="C478" s="9"/>
       <c r="D478" s="9"/>
       <c r="E478" s="9"/>
-      <c r="F478" s="9"/>
+      <c r="F478" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G478" s="9"/>
       <c r="H478" s="9"/>
       <c r="I478" s="14"/>
@@ -7890,7 +8234,9 @@
       <c r="C479" s="9"/>
       <c r="D479" s="9"/>
       <c r="E479" s="9"/>
-      <c r="F479" s="9"/>
+      <c r="F479" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G479" s="9"/>
       <c r="H479" s="9"/>
       <c r="I479" s="14"/>
@@ -7904,7 +8250,9 @@
       <c r="C480" s="9"/>
       <c r="D480" s="9"/>
       <c r="E480" s="9"/>
-      <c r="F480" s="9"/>
+      <c r="F480" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G480" s="9"/>
       <c r="H480" s="9"/>
       <c r="I480" s="14"/>
@@ -7918,7 +8266,9 @@
       <c r="C481" s="9"/>
       <c r="D481" s="9"/>
       <c r="E481" s="9"/>
-      <c r="F481" s="9"/>
+      <c r="F481" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G481" s="9"/>
       <c r="H481" s="9"/>
       <c r="I481" s="14"/>
@@ -7932,7 +8282,9 @@
       <c r="C482" s="9"/>
       <c r="D482" s="9"/>
       <c r="E482" s="9"/>
-      <c r="F482" s="9"/>
+      <c r="F482" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G482" s="9"/>
       <c r="H482" s="9"/>
       <c r="I482" s="14"/>
@@ -7946,7 +8298,9 @@
       <c r="C483" s="9"/>
       <c r="D483" s="9"/>
       <c r="E483" s="9"/>
-      <c r="F483" s="9"/>
+      <c r="F483" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G483" s="9"/>
       <c r="H483" s="9"/>
       <c r="I483" s="14"/>
@@ -7960,7 +8314,9 @@
       <c r="C484" s="9"/>
       <c r="D484" s="9"/>
       <c r="E484" s="9"/>
-      <c r="F484" s="9"/>
+      <c r="F484" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G484" s="9"/>
       <c r="H484" s="9"/>
       <c r="I484" s="14"/>
@@ -7974,7 +8330,9 @@
       <c r="C485" s="9"/>
       <c r="D485" s="9"/>
       <c r="E485" s="9"/>
-      <c r="F485" s="9"/>
+      <c r="F485" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G485" s="9"/>
       <c r="H485" s="9"/>
       <c r="I485" s="14"/>
@@ -7988,7 +8346,9 @@
       <c r="C486" s="9"/>
       <c r="D486" s="9"/>
       <c r="E486" s="9"/>
-      <c r="F486" s="9"/>
+      <c r="F486" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G486" s="9"/>
       <c r="H486" s="9"/>
       <c r="I486" s="14"/>
@@ -8002,7 +8362,9 @@
       <c r="C487" s="9"/>
       <c r="D487" s="9"/>
       <c r="E487" s="9"/>
-      <c r="F487" s="9"/>
+      <c r="F487" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G487" s="9"/>
       <c r="H487" s="9"/>
       <c r="I487" s="14"/>
@@ -8016,7 +8378,9 @@
       <c r="C488" s="9"/>
       <c r="D488" s="9"/>
       <c r="E488" s="9"/>
-      <c r="F488" s="9"/>
+      <c r="F488" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G488" s="9"/>
       <c r="H488" s="9"/>
       <c r="I488" s="14"/>
@@ -8030,7 +8394,9 @@
       <c r="C489" s="9"/>
       <c r="D489" s="9"/>
       <c r="E489" s="9"/>
-      <c r="F489" s="9"/>
+      <c r="F489" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G489" s="9"/>
       <c r="H489" s="9"/>
       <c r="I489" s="14"/>
@@ -8044,7 +8410,9 @@
       <c r="C490" s="9"/>
       <c r="D490" s="9"/>
       <c r="E490" s="9"/>
-      <c r="F490" s="9"/>
+      <c r="F490" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G490" s="9"/>
       <c r="H490" s="9"/>
       <c r="I490" s="14"/>
@@ -8058,7 +8426,9 @@
       <c r="C491" s="9"/>
       <c r="D491" s="9"/>
       <c r="E491" s="9"/>
-      <c r="F491" s="9"/>
+      <c r="F491" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G491" s="9"/>
       <c r="H491" s="9"/>
       <c r="I491" s="14"/>
@@ -8072,7 +8442,9 @@
       <c r="C492" s="9"/>
       <c r="D492" s="9"/>
       <c r="E492" s="9"/>
-      <c r="F492" s="9"/>
+      <c r="F492" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G492" s="9"/>
       <c r="H492" s="9"/>
       <c r="I492" s="14"/>
@@ -8086,7 +8458,9 @@
       <c r="C493" s="9"/>
       <c r="D493" s="9"/>
       <c r="E493" s="9"/>
-      <c r="F493" s="9"/>
+      <c r="F493" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G493" s="9"/>
       <c r="H493" s="9"/>
       <c r="I493" s="14"/>
@@ -8100,7 +8474,9 @@
       <c r="C494" s="9"/>
       <c r="D494" s="9"/>
       <c r="E494" s="9"/>
-      <c r="F494" s="9"/>
+      <c r="F494" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G494" s="9"/>
       <c r="H494" s="9"/>
       <c r="I494" s="14"/>
@@ -8114,7 +8490,9 @@
       <c r="C495" s="9"/>
       <c r="D495" s="9"/>
       <c r="E495" s="9"/>
-      <c r="F495" s="9"/>
+      <c r="F495" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G495" s="9"/>
       <c r="H495" s="9"/>
       <c r="I495" s="14"/>
@@ -8128,7 +8506,9 @@
       <c r="C496" s="9"/>
       <c r="D496" s="9"/>
       <c r="E496" s="9"/>
-      <c r="F496" s="9"/>
+      <c r="F496" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G496" s="9"/>
       <c r="H496" s="9"/>
       <c r="I496" s="14"/>
@@ -8142,7 +8522,9 @@
       <c r="C497" s="9"/>
       <c r="D497" s="9"/>
       <c r="E497" s="9"/>
-      <c r="F497" s="9"/>
+      <c r="F497" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G497" s="9"/>
       <c r="H497" s="9"/>
       <c r="I497" s="14"/>
@@ -8156,7 +8538,9 @@
       <c r="C498" s="9"/>
       <c r="D498" s="9"/>
       <c r="E498" s="9"/>
-      <c r="F498" s="9"/>
+      <c r="F498" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G498" s="9"/>
       <c r="H498" s="9"/>
       <c r="I498" s="14"/>
@@ -8170,7 +8554,9 @@
       <c r="C499" s="9"/>
       <c r="D499" s="9"/>
       <c r="E499" s="9"/>
-      <c r="F499" s="9"/>
+      <c r="F499" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G499" s="9"/>
       <c r="H499" s="9"/>
       <c r="I499" s="14"/>
@@ -8184,7 +8570,9 @@
       <c r="C500" s="9"/>
       <c r="D500" s="9"/>
       <c r="E500" s="9"/>
-      <c r="F500" s="9"/>
+      <c r="F500" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G500" s="9"/>
       <c r="H500" s="9"/>
       <c r="I500" s="14"/>
@@ -8198,7 +8586,9 @@
       <c r="C501" s="9"/>
       <c r="D501" s="9"/>
       <c r="E501" s="9"/>
-      <c r="F501" s="9"/>
+      <c r="F501" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G501" s="9"/>
       <c r="H501" s="9"/>
       <c r="I501" s="14"/>
@@ -8212,7 +8602,9 @@
       <c r="C502" s="9"/>
       <c r="D502" s="9"/>
       <c r="E502" s="9"/>
-      <c r="F502" s="9"/>
+      <c r="F502" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G502" s="9"/>
       <c r="H502" s="9"/>
       <c r="I502" s="14"/>
@@ -8226,7 +8618,9 @@
       <c r="C503" s="9"/>
       <c r="D503" s="9"/>
       <c r="E503" s="9"/>
-      <c r="F503" s="9"/>
+      <c r="F503" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G503" s="9"/>
       <c r="H503" s="9"/>
       <c r="I503" s="14"/>
@@ -8240,7 +8634,9 @@
       <c r="C504" s="9"/>
       <c r="D504" s="9"/>
       <c r="E504" s="9"/>
-      <c r="F504" s="9"/>
+      <c r="F504" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G504" s="9"/>
       <c r="H504" s="9"/>
       <c r="I504" s="14"/>
@@ -8254,7 +8650,9 @@
       <c r="C505" s="9"/>
       <c r="D505" s="9"/>
       <c r="E505" s="9"/>
-      <c r="F505" s="9"/>
+      <c r="F505" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G505" s="9"/>
       <c r="H505" s="9"/>
       <c r="I505" s="14"/>
@@ -12074,10 +12472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12086,7 +12484,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -12095,7 +12493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -12104,7 +12502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -12113,7 +12511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -12122,7 +12520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -12131,43 +12529,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="6">
         <f>COUNTA(Feuil1!F3:F425)</f>
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="6">
         <f>COUNTIF(Feuil1!F3:F425,"OK")</f>
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="6">
         <f>COUNTIF(Feuil1!F3:F425,"gain")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6">
         <f>COUNTIF(Feuil1!F3:F425,"noise")</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -12176,28 +12574,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B14">
         <f>COUNTIF(Feuil1!F3:F425,"POWER")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>SUM(B10:B14)</f>
-        <v>301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="C15" s="17">
+        <f>B10/B15</f>
+        <v>0.89834515366430256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6">
         <f>COUNTIF(Feuil1!F1:F425,"TODO")</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>